<commit_message>
Updates to lab report
</commit_message>
<xml_diff>
--- a/Y3 Lab/Plots/calib20121108.xlsx
+++ b/Y3 Lab/Plots/calib20121108.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" tabRatio="862" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -15,14 +15,19 @@
     <sheet name="Efficiency NaI" sheetId="3" r:id="rId6"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId7"/>
     <sheet name="Chart2" sheetId="10" r:id="rId8"/>
-    <sheet name="Efficiency BF3" sheetId="8" r:id="rId9"/>
+    <sheet name="Advanced calibration" sheetId="11" r:id="rId9"/>
+    <sheet name="Advanced calibration (2)" sheetId="12" r:id="rId10"/>
+    <sheet name="Chart3" sheetId="13" r:id="rId11"/>
+    <sheet name="Chart4" sheetId="14" r:id="rId12"/>
+    <sheet name="Efficiency BF3" sheetId="8" r:id="rId13"/>
+    <sheet name="Solver 2group BF3" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
   <si>
     <t>Channel Number</t>
   </si>
@@ -116,12 +121,60 @@
   <si>
     <t>Counts-Backgnd</t>
   </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Differences</t>
+  </si>
+  <si>
+    <t>Error on Differences</t>
+  </si>
+  <si>
+    <t>Error on Energy</t>
+  </si>
+  <si>
+    <t>Error on Chn</t>
+  </si>
+  <si>
+    <t>Counts x r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                 </t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>taut</t>
+  </si>
+  <si>
+    <t>Lt</t>
+  </si>
+  <si>
+    <t>χ</t>
+  </si>
+  <si>
+    <t>Dbar</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Chi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,16 +188,56 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,21 +245,163 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="11" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -311,11 +546,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98117504"/>
-        <c:axId val="98824192"/>
+        <c:axId val="44499712"/>
+        <c:axId val="44501632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98117504"/>
+        <c:axId val="44499712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="400"/>
@@ -340,18 +575,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98824192"/>
+        <c:crossAx val="44501632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98824192"/>
+        <c:axId val="44501632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1500"/>
@@ -376,13 +612,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98117504"/>
+        <c:crossAx val="44499712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -391,6 +628,616 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11531218558261783"/>
+                  <c:y val="-3.2435563278308717E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Efficiency BF3'!$A$5:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Efficiency BF3'!$K$5:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.514786320738969</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.320327169987438</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.103820044841459</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.875872131800394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.630782296011775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.353734000952977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.090617686432669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8167869465035391</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5462676758347786</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="137392896"/>
+        <c:axId val="137394432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="137392896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>r</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (m)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="137394432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="137394432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ln(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR">
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>φ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB">
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>r)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="137392896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Efficiency BF3'!$A$3:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Efficiency BF3'!$L$3:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>278157.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>282406.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>255474.96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210327.37600000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>169382.272</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>134856.35999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>105543.20300000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80003.635800000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61494.993600000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46764.5308</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35680.551200000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="97924224"/>
+        <c:axId val="125202816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="97924224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="125202816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="125202816"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="97924224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.743941098271807E-2"/>
+                  <c:y val="-6.6835502987968309E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Efficiency BF3'!$A$5:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Efficiency BF3'!$K$5:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>11.514786320738969</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.320327169987438</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.103820044841459</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.875872131800394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.630782296011775</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.353734000952977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.090617686432669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8167869465035391</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5462676758347786</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="95988352"/>
+        <c:axId val="96126464"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="95988352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Radius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96126464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="96126464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" vert="horz"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="95988352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -534,11 +1381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100423552"/>
-        <c:axId val="100432896"/>
+        <c:axId val="46734720"/>
+        <c:axId val="46736896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100423552"/>
+        <c:axId val="46734720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.5"/>
@@ -561,18 +1408,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100432896"/>
+        <c:crossAx val="46736896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100432896"/>
+        <c:axId val="46736896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-1.5"/>
@@ -596,13 +1444,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100423552"/>
+        <c:crossAx val="46734720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -730,11 +1579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95820800"/>
-        <c:axId val="95822592"/>
+        <c:axId val="47126016"/>
+        <c:axId val="47127552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95820800"/>
+        <c:axId val="47126016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -744,12 +1593,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95822592"/>
+        <c:crossAx val="47127552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95822592"/>
+        <c:axId val="47127552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +1609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95820800"/>
+        <c:crossAx val="47126016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -893,11 +1742,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95838208"/>
-        <c:axId val="95839744"/>
+        <c:axId val="47173632"/>
+        <c:axId val="47175168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95838208"/>
+        <c:axId val="47173632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="5.5"/>
@@ -908,12 +1757,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95839744"/>
+        <c:crossAx val="47175168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95839744"/>
+        <c:axId val="47175168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,7 +1773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95838208"/>
+        <c:crossAx val="47173632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1071,11 +1920,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95847936"/>
-        <c:axId val="95849856"/>
+        <c:axId val="46803200"/>
+        <c:axId val="46817664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95847936"/>
+        <c:axId val="46803200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1097,18 +1946,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95849856"/>
+        <c:crossAx val="46817664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95849856"/>
+        <c:axId val="46817664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1139,13 +1989,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95847936"/>
+        <c:crossAx val="46803200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1273,11 +2124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95862144"/>
-        <c:axId val="98088064"/>
+        <c:axId val="46915584"/>
+        <c:axId val="46917120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95862144"/>
+        <c:axId val="46915584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1287,12 +2138,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98088064"/>
+        <c:crossAx val="46917120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98088064"/>
+        <c:axId val="46917120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,13 +2154,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95862144"/>
+        <c:crossAx val="46915584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1402,37 +2254,22 @@
                 <c:pt idx="10">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.12</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.2</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.26</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>0.28000000000000003</c:v>
                 </c:pt>
               </c:numCache>
@@ -1477,38 +2314,23 @@
                 <c:pt idx="10">
                   <c:v>127430.54</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>3466389</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>2816956</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>994868</c:v>
+                  <c:v>123920.85</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1485785.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>731297</c:v>
+                  <c:v>63365.7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>525283.125</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>386557.5</c:v>
+                  <c:v>28428.62</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>251766.965</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>257180.375</c:v>
+                  <c:v>13879.475</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>128904.66</c:v>
+                  <c:v>6528.93</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3324.13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1523,16 +2345,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98129024"/>
-        <c:axId val="98130944"/>
+        <c:axId val="47017984"/>
+        <c:axId val="47019904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98129024"/>
+        <c:axId val="47017984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1549,18 +2372,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98130944"/>
+        <c:crossAx val="47019904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98130944"/>
+        <c:axId val="47019904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,13 +2407,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98129024"/>
+        <c:crossAx val="47017984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1615,6 +2440,10 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1624,6 +2453,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Advanced calibration (2)'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>155.50</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -1631,84 +2471,48 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>'Efficiency BF3'!$H$3:$H$13</c:f>
+              <c:f>'Advanced calibration (2)'!$B$3:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3476970.5</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2824068</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2128958</c:v>
+                  <c:v>1157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1502338.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1058639.2</c:v>
+                  <c:v>1449</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>749202</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>527716.01500000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>363652.89</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256229.14</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>179863.58</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>127430.54</c:v>
+                  <c:v>2656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Efficiency BF3'!$K$3:$K$13</c:f>
+              <c:f>'Advanced calibration (2)'!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>-6.381649804751941E-3</c:v>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>202.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.967426697006617E-3</c:v>
+                  <c:v>445.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.6378732334576785E-3</c:v>
+                  <c:v>346.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.1422584568385434E-2</c:v>
+                  <c:v>564</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.3289132125043917E-2</c:v>
+                  <c:v>648.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.5238784784597881E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1.7290753870116811E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.9486569013186138E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-2.1765329571749509E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-2.4179567949139006E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-2.671153941988447E-2</c:v>
+                  <c:v>700.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1723,37 +2527,37 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="3333120"/>
-        <c:axId val="3334912"/>
+        <c:axId val="121126272"/>
+        <c:axId val="121124736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3333120"/>
+        <c:axId val="121126272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3334912"/>
+        <c:crossAx val="121124736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3334912"/>
+        <c:axId val="121124736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3333120"/>
+        <c:crossAx val="121126272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1803,6 +2607,11 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Efficiency BF3'!$A$3:$A$13</c:f>
@@ -1847,7 +2656,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Efficiency BF3'!$I$3:$I$13</c:f>
+              <c:f>'Efficiency BF3'!$L$3:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1897,55 +2706,92 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="168890752"/>
-        <c:axId val="168892288"/>
+        <c:axId val="137426432"/>
+        <c:axId val="137427968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168890752"/>
+        <c:axId val="137426432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Radius (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168892288"/>
+        <c:crossAx val="137427968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168892288"/>
+        <c:axId val="137427968"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Ln(Counts</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> x Radius)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168890752"/>
+        <c:crossAx val="137426432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="10"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1977,7 +2823,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="203" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="202" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
@@ -1989,10 +2835,35 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="203" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="203" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="203" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -2023,11 +2894,60 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="9172575" y="2819399"/>
+    <xdr:ext cx="9658350" cy="4207761"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="10639425" y="2428875"/>
+    <xdr:ext cx="8820150" cy="4960236"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6167673" cy="3843007"/>
+    <xdr:ext cx="6167673" cy="3857153"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2121,7 +3041,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="6165443" cy="3842845"/>
+    <xdr:ext cx="6167673" cy="3857153"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2185,7 +3105,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:ext cx="6991256" cy="3842845"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -2212,20 +3132,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2240,23 +3160,20 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:to>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6991256" cy="3842845"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2264,13 +3181,109 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6991256" cy="3842845"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F10" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:F10"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Channel"/>
+    <tableColumn id="2" name="Error on Chn" dataDxfId="16"/>
+    <tableColumn id="3" name="Energy" dataDxfId="15">
+      <calculatedColumnFormula>(A2*3.035)-54</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Error on Energy" dataDxfId="14">
+      <calculatedColumnFormula>SQRT((B2*3.035)^2+(0.05*A2)^2+(30)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Differences" dataDxfId="13">
+      <calculatedColumnFormula>C2-C1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Error on Differences" dataDxfId="12">
+      <calculatedColumnFormula>(D2^2+D1^2)^0.5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A18:F27" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A18:F27"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Channel"/>
+    <tableColumn id="2" name="Error on Chn" dataDxfId="10"/>
+    <tableColumn id="3" name="Energy" dataDxfId="9">
+      <calculatedColumnFormula>(A19*3.035)-54</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Error on Energy" dataDxfId="8">
+      <calculatedColumnFormula>SQRT((B19*3.035)^2+(0.05*A19)^2+(30)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Differences" dataDxfId="7">
+      <calculatedColumnFormula>C19-C18</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Error on Differences" dataDxfId="6">
+      <calculatedColumnFormula>(D19^2+D18^2)^0.5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="C1:H10" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="C1:H10"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Channel"/>
+    <tableColumn id="2" name="Error on Chn" dataDxfId="4"/>
+    <tableColumn id="3" name="Energy" dataDxfId="3">
+      <calculatedColumnFormula>(C2*3.035)-54</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Error on Energy" dataDxfId="2">
+      <calculatedColumnFormula>SQRT((D2*3.035)^2+(0.05*C2)^2+(30)^2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="Differences" dataDxfId="1">
+      <calculatedColumnFormula>E2-E1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Error on Differences" dataDxfId="0">
+      <calculatedColumnFormula>(F2^2+F1^2)^0.5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3068,7 +4081,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="B20" sqref="B20:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4375,10 +5388,764 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K1048576"/>
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>181.20400000000001</v>
+      </c>
+      <c r="B2" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <f>(A2*3.035)-54</f>
+        <v>495.95414000000005</v>
+      </c>
+      <c r="D2" s="4">
+        <f>SQRT((B2*3.035)^2+(0.05*A2)^2+(30)^2)</f>
+        <v>31.338991034213272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>232.45</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C10" si="0">(A3*3.035)-54</f>
+        <v>651.48575000000005</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D10" si="1">SQRT((B3*3.035)^2+(0.05*A3)^2+(30)^2)</f>
+        <v>32.172755411061701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>403.33</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>1170.10655</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>36.151002403979064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>458.6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>1337.8510000000001</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="1"/>
+        <v>37.763518687881827</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>617.29999999999995</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>1819.5055</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="1"/>
+        <v>43.075942997919384</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" ref="E6:E8" si="2">C6-C5</f>
+        <v>481.65449999999987</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" ref="F6:F8" si="3">(D6^2+D5^2)^0.5</f>
+        <v>57.285427543573419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>757.2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>2244.1020000000003</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="1"/>
+        <v>48.305678256701874</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="2"/>
+        <v>424.59650000000033</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="3"/>
+        <v>64.722294590040619</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1168.5</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>3492.3975</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="1"/>
+        <v>65.795498290156601</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="2"/>
+        <v>1248.2954999999997</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="3"/>
+        <v>81.624053728603798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1335.4</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>3998.9390000000003</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>73.21567937436626</v>
+      </c>
+      <c r="E9" s="4">
+        <f>C9-C8</f>
+        <v>506.54150000000027</v>
+      </c>
+      <c r="F9" s="4">
+        <f>(D9^2+D8^2)^0.5</f>
+        <v>98.435681038432406</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1496.6</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>4488.1809999999996</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>80.624134476222437</v>
+      </c>
+      <c r="E10" s="4">
+        <f>C10-C9</f>
+        <v>489.24199999999928</v>
+      </c>
+      <c r="F10" s="4">
+        <f>(D10^2+D9^2)^0.5</f>
+        <v>108.90723927402622</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>181.20400000000001</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C19" s="4">
+        <f>(A19*3.035)-54</f>
+        <v>495.95414000000005</v>
+      </c>
+      <c r="D19" s="4">
+        <f>SQRT((B19*3.035)^2+(0.05*A19)^2+(30)^2)</f>
+        <v>31.338991034213272</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>232.45</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" ref="C20:C27" si="4">(A20*3.035)-54</f>
+        <v>651.48575000000005</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" ref="D20:D27" si="5">SQRT((B20*3.035)^2+(0.05*A20)^2+(30)^2)</f>
+        <v>32.172755411061701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>403.33</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="4"/>
+        <v>1170.10655</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="5"/>
+        <v>36.151002403979064</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>458.6</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="4"/>
+        <v>1337.8510000000001</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="5"/>
+        <v>37.763518687881827</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>617.29999999999995</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="4"/>
+        <v>1819.5055</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="5"/>
+        <v>43.075942997919384</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" ref="E23:E25" si="6">C23-C22</f>
+        <v>481.65449999999987</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" ref="F23:F25" si="7">(D23^2+D22^2)^0.5</f>
+        <v>57.285427543573419</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>757.2</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="4"/>
+        <v>2244.1020000000003</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="5"/>
+        <v>48.305678256701874</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" si="6"/>
+        <v>424.59650000000033</v>
+      </c>
+      <c r="F24" s="4">
+        <f t="shared" si="7"/>
+        <v>64.722294590040619</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1168.5</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="4"/>
+        <v>3492.3975</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="5"/>
+        <v>65.795498290156601</v>
+      </c>
+      <c r="E25" s="4">
+        <f t="shared" si="6"/>
+        <v>1248.2954999999997</v>
+      </c>
+      <c r="F25" s="4">
+        <f t="shared" si="7"/>
+        <v>81.624053728603798</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1335.4</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="4"/>
+        <v>3998.9390000000003</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="5"/>
+        <v>73.21567937436626</v>
+      </c>
+      <c r="E26" s="4">
+        <f>C26-C25</f>
+        <v>506.54150000000027</v>
+      </c>
+      <c r="F26" s="4">
+        <f>(D26^2+D25^2)^0.5</f>
+        <v>98.435681038432406</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1496.6</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="4"/>
+        <v>4488.1809999999996</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="5"/>
+        <v>80.624134476222437</v>
+      </c>
+      <c r="E27" s="4">
+        <f>C27-C26</f>
+        <v>489.24199999999928</v>
+      </c>
+      <c r="F27" s="4">
+        <f>(D27^2+D26^2)^0.5</f>
+        <v>108.90723927402622</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="C2" activeCellId="1" sqref="B2:B8 C2:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6">
+        <v>155.5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E2" s="4">
+        <f>(C2*3.035)-54</f>
+        <v>417.9425</v>
+      </c>
+      <c r="F2" s="4">
+        <f>SQRT((D2*3.035)^2+(0.05*C2)^2+(30)^2)</f>
+        <v>30.994481404961434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>511</v>
+      </c>
+      <c r="C3" s="6">
+        <v>202.12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E10" si="0">(C3*3.035)-54</f>
+        <v>559.43420000000003</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" ref="F3:F10" si="1">SQRT((D3*3.035)^2+(0.05*C3)^2+(30)^2)</f>
+        <v>31.656481053601411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>1157</v>
+      </c>
+      <c r="C4">
+        <v>445.54</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>1298.2139000000002</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>37.366934006719099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>346.2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>996.7170000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="1"/>
+        <v>34.639606008188082</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>1449</v>
+      </c>
+      <c r="C6">
+        <v>564</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>1657.74</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>41.334055740998849</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" ref="G6:G8" si="2">E6-E5</f>
+        <v>661.02299999999991</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:H8" si="3">(F6^2+F5^2)^0.5</f>
+        <v>53.929643688814593</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>648.5</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>1914.1975</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>44.225491803370602</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="2"/>
+        <v>256.45749999999998</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="3"/>
+        <v>60.534273674093093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>2656</v>
+      </c>
+      <c r="C8">
+        <v>700.9</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>2073.2314999999999</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="1"/>
+        <v>46.147869084064979</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="2"/>
+        <v>159.03399999999988</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="3"/>
+        <v>63.918072141218403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>-54</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G9" s="4">
+        <f>E9-E8</f>
+        <v>-2127.2314999999999</v>
+      </c>
+      <c r="H9" s="4">
+        <f>(F9^2+F8^2)^0.5</f>
+        <v>55.042036853663035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="6"/>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>-54</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G10" s="4">
+        <f>E10-E9</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <f>(F10^2+F9^2)^0.5</f>
+        <v>42.426406871192853</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="6"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="6"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="6"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="6"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="6"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="6"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="6"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N1048576"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4390,12 +6157,13 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>26</v>
       </c>
@@ -4417,8 +6185,11 @@
       <c r="H2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.08</v>
       </c>
@@ -4446,19 +6217,30 @@
         <v>3476970.5</v>
       </c>
       <c r="I3" s="1">
+        <f>H3/(600*(0.17*0.025))</f>
+        <v>1363517.8431372547</v>
+      </c>
+      <c r="J3" s="1">
+        <f>I3*A3</f>
+        <v>109081.42745098038</v>
+      </c>
+      <c r="K3" s="1">
+        <f>LN(J3)</f>
+        <v>11.599849923149849</v>
+      </c>
+      <c r="L3" s="1">
         <f>H3*A3</f>
         <v>278157.64</v>
       </c>
-      <c r="J3">
-        <f>LN(I3)</f>
-        <v>12.535943282320183</v>
-      </c>
-      <c r="K3">
-        <f>-A3/J3</f>
-        <v>-6.381649804751941E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="e">
+        <f>-A3/M3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -4475,7 +6257,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F25" si="0">0.5*(C4+E4)*(D4-B4)</f>
+        <f t="shared" ref="F4:F13" si="0">0.5*(C4+E4)*(D4-B4)</f>
         <v>275132</v>
       </c>
       <c r="G4" s="1">
@@ -4486,19 +6268,31 @@
         <v>2824068</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I13" si="1">H4*A4</f>
+        <f t="shared" ref="I4:I13" si="1">H4/(600*(0.17*0.025))</f>
+        <v>1107477.6470588234</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J13" si="2">I4*A4</f>
+        <v>110747.76470588235</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K13" si="3">LN(J4)</f>
+        <v>11.6150105044611</v>
+      </c>
+      <c r="L4" s="1">
+        <f>H4*A4</f>
         <v>282406.8</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J13" si="2">LN(I4)</f>
+      <c r="M4">
+        <f t="shared" ref="M4:M13" si="4">LN(L4)</f>
         <v>12.551103863631436</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K13" si="3">-A4/J4</f>
+      <c r="N4">
+        <f>-A4/M4</f>
         <v>-7.967426697006617E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.12</v>
       </c>
@@ -4527,18 +6321,30 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
+        <v>834885.49019607832</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>100186.2588235294</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>11.514786320738969</v>
+      </c>
+      <c r="L5" s="1">
+        <f>H5*A5</f>
         <v>255474.96</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
+      <c r="M5">
+        <f t="shared" si="4"/>
         <v>12.450879679909304</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
+      <c r="N5">
+        <f>-A5/M5</f>
         <v>-9.6378732334576785E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.14000000000000001</v>
       </c>
@@ -4562,23 +6368,35 @@
         <v>1643000</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:H25" si="4">G6-F6</f>
+        <f t="shared" ref="H6:H25" si="5">G6-F6</f>
         <v>1502338.4</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
+        <v>589152.31372549012</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>82481.323921568619</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="3"/>
+        <v>11.320327169987438</v>
+      </c>
+      <c r="L6" s="1">
+        <f>H6*A6</f>
         <v>210327.37600000002</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
+      <c r="M6">
+        <f t="shared" si="4"/>
         <v>12.256420529157774</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
+      <c r="N6">
+        <f>-A6/M6</f>
         <v>-1.1422584568385434E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.16</v>
       </c>
@@ -4602,23 +6420,35 @@
         <v>1156000</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1058639.2</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
+        <v>415152.6274509803</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="2"/>
+        <v>66424.420392156855</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>11.103820044841459</v>
+      </c>
+      <c r="L7" s="1">
+        <f>H7*A7</f>
         <v>169382.272</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
+      <c r="M7">
+        <f t="shared" si="4"/>
         <v>12.039913404011795</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
+      <c r="N7">
+        <f>-A7/M7</f>
         <v>-1.3289132125043917E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.18</v>
       </c>
@@ -4642,23 +6472,35 @@
         <v>817782</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>749202</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
+        <v>293804.70588235289</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="2"/>
+        <v>52884.847058823521</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>10.875872131800394</v>
+      </c>
+      <c r="L8" s="1">
+        <f>H8*A8</f>
         <v>134856.35999999999</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
+      <c r="M8">
+        <f t="shared" si="4"/>
         <v>11.81196549097073</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
+      <c r="N8">
+        <f>-A8/M8</f>
         <v>-1.5238784784597881E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.2</v>
       </c>
@@ -4682,23 +6524,35 @@
         <v>575845</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>527716.01500000001</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
+        <v>206947.45686274508</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="2"/>
+        <v>41389.491372549019</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="3"/>
+        <v>10.630782296011775</v>
+      </c>
+      <c r="L9" s="1">
+        <f>H9*A9</f>
         <v>105543.20300000001</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
+      <c r="M9">
+        <f t="shared" si="4"/>
         <v>11.566875655182111</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="3"/>
+      <c r="N9">
+        <f>-A9/M9</f>
         <v>-1.7290753870116811E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.22</v>
       </c>
@@ -4722,23 +6576,35 @@
         <v>397794</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>363652.89</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
+        <v>142608.97647058821</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="2"/>
+        <v>31373.974823529406</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="3"/>
+        <v>10.353734000952977</v>
+      </c>
+      <c r="L10" s="1">
+        <f>H10*A10</f>
         <v>80003.635800000004</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
+      <c r="M10">
+        <f t="shared" si="4"/>
         <v>11.289827360123313</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="3"/>
+      <c r="N10">
+        <f>-A10/M10</f>
         <v>-1.9486569013186138E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.24</v>
       </c>
@@ -4762,23 +6628,35 @@
         <v>280046</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>256229.14</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
+        <v>100482.01568627451</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="2"/>
+        <v>24115.683764705882</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>10.090617686432669</v>
+      </c>
+      <c r="L11" s="1">
+        <f>H11*A11</f>
         <v>61494.993600000002</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
+      <c r="M11">
+        <f t="shared" si="4"/>
         <v>11.026711045603003</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="3"/>
+      <c r="N11">
+        <f>-A11/M11</f>
         <v>-2.1765329571749509E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.26</v>
       </c>
@@ -4802,23 +6680,35 @@
         <v>196834</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>179863.58</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
+        <v>70534.737254901949</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="2"/>
+        <v>18339.031686274506</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>9.8167869465035391</v>
+      </c>
+      <c r="L12" s="1">
+        <f>H12*A12</f>
         <v>46764.5308</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
+      <c r="M12">
+        <f t="shared" si="4"/>
         <v>10.752880305673873</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="3"/>
+      <c r="N12">
+        <f>-A12/M12</f>
         <v>-2.4179567949139006E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.28000000000000003</v>
       </c>
@@ -4842,324 +6732,588 @@
         <v>139580</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>127430.54</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
+        <v>49972.760784313716</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>13992.373019607841</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="3"/>
+        <v>9.5462676758347786</v>
+      </c>
+      <c r="L13" s="1">
+        <f>H13*A13</f>
         <v>35680.551200000002</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
+      <c r="M13">
+        <f t="shared" si="4"/>
         <v>10.482361035005113</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="3"/>
+      <c r="N13">
+        <f>-A13/M13</f>
         <v>-2.671153941988447E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>0.08</v>
       </c>
-      <c r="B15" s="4">
-        <v>403</v>
-      </c>
-      <c r="C15" s="1">
-        <v>490</v>
-      </c>
-      <c r="D15">
-        <v>1717</v>
-      </c>
-      <c r="E15">
-        <v>33</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>343611</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3810000</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="4"/>
-        <v>3466389</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0.1</v>
-      </c>
       <c r="B16" s="4">
-        <v>399</v>
+        <v>451</v>
       </c>
       <c r="C16" s="1">
-        <v>390</v>
+        <v>25</v>
       </c>
       <c r="D16">
-        <v>1773</v>
+        <v>1862</v>
       </c>
       <c r="E16">
-        <v>22</v>
+        <v>0.3</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>283044</v>
+        <f>0.5*(C16+E16)*(D16-B16)</f>
+        <v>17849.150000000001</v>
       </c>
       <c r="G16" s="1">
-        <v>3100000</v>
+        <v>141770</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="4"/>
-        <v>2816956</v>
+        <f>G16-F16</f>
+        <v>123920.85</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0.12</v>
-      </c>
-      <c r="B17" s="4">
-        <v>389</v>
-      </c>
-      <c r="C17" s="1">
-        <v>290</v>
-      </c>
-      <c r="D17">
-        <v>1677</v>
-      </c>
-      <c r="E17">
-        <v>13</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>195132</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1190000</v>
-      </c>
-      <c r="H17" s="1">
-        <f t="shared" si="4"/>
-        <v>994868</v>
-      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="B18" s="4">
-        <v>399</v>
+        <v>432</v>
       </c>
       <c r="C18" s="1">
-        <v>210</v>
+        <v>13</v>
       </c>
       <c r="D18">
-        <v>1636</v>
+        <v>1858</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>0.1</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>134214.5</v>
+        <f>0.5*(C18+E18)*(D18-B18)</f>
+        <v>9340.2999999999993</v>
       </c>
       <c r="G18" s="1">
-        <v>1620000</v>
+        <v>72706</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="4"/>
-        <v>1485785.5</v>
+        <f>G18-F18</f>
+        <v>63365.7</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0.16</v>
-      </c>
-      <c r="B19" s="4">
-        <v>391</v>
-      </c>
-      <c r="C19" s="1">
-        <v>110</v>
-      </c>
-      <c r="D19">
-        <v>1676</v>
-      </c>
-      <c r="E19">
-        <v>1.6</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>71703</v>
-      </c>
-      <c r="G19" s="1">
-        <v>803000</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="4"/>
-        <v>731297</v>
-      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="B20" s="4">
-        <v>397</v>
+        <v>462</v>
       </c>
       <c r="C20" s="1">
-        <v>74</v>
+        <v>5.5</v>
       </c>
       <c r="D20">
-        <v>1672</v>
+        <v>1856</v>
       </c>
       <c r="E20">
-        <v>0.85</v>
+        <v>0.04</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>47716.875</v>
+        <f>0.5*(C20+E20)*(D20-B20)</f>
+        <v>3861.38</v>
       </c>
       <c r="G20" s="1">
-        <v>573000</v>
+        <v>32290</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="4"/>
-        <v>525283.125</v>
+        <f>G20-F20</f>
+        <v>28428.62</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>0.2</v>
-      </c>
-      <c r="B21" s="4">
-        <v>388</v>
-      </c>
-      <c r="C21" s="1">
-        <v>56</v>
-      </c>
-      <c r="D21">
-        <v>1678</v>
-      </c>
-      <c r="E21">
-        <v>0.5</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>36442.5</v>
-      </c>
-      <c r="G21" s="1">
-        <v>423000</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" si="4"/>
-        <v>386557.5</v>
-      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="B22" s="4">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="C22" s="1">
-        <v>36</v>
+        <v>2.6</v>
       </c>
       <c r="D22">
-        <v>1668</v>
+        <v>1849</v>
       </c>
       <c r="E22">
-        <v>0.33</v>
+        <v>0.05</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>23233.035</v>
+        <f>0.5*(C22+E22)*(D22-B22)</f>
+        <v>1877.5249999999999</v>
       </c>
       <c r="G22" s="1">
-        <v>275000</v>
+        <v>15757</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="4"/>
-        <v>251766.965</v>
+        <f>G22-F22</f>
+        <v>13879.475</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0.24</v>
-      </c>
-      <c r="B23" s="4">
-        <v>396</v>
-      </c>
-      <c r="C23" s="1">
-        <v>35</v>
-      </c>
-      <c r="D23">
-        <v>1677</v>
-      </c>
-      <c r="E23">
-        <v>0.25</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>22577.625</v>
-      </c>
-      <c r="G23" s="1">
-        <v>279758</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="4"/>
-        <v>257180.375</v>
-      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0.26</v>
+        <v>0.24</v>
+      </c>
+      <c r="B24" s="4">
+        <v>457</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D24">
+        <v>1831</v>
+      </c>
+      <c r="E24">
+        <v>0.01</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>0.5*(C24+E24)*(D24-B24)</f>
+        <v>1106.0700000000002</v>
+      </c>
+      <c r="G24" s="1">
+        <v>7635</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>G24-F24</f>
+        <v>6528.93</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="F25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>0.28000000000000003</v>
       </c>
-      <c r="B25" s="4">
-        <v>397</v>
-      </c>
-      <c r="C25" s="1">
-        <v>18</v>
-      </c>
-      <c r="D25">
-        <v>1659</v>
-      </c>
-      <c r="E25">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="0"/>
-        <v>11446.34</v>
-      </c>
-      <c r="G25" s="1">
-        <v>140351</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="4"/>
-        <v>128904.66</v>
-      </c>
-    </row>
-    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>453</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D26">
+        <v>1847</v>
+      </c>
+      <c r="E26">
+        <v>0.01</v>
+      </c>
+      <c r="F26" s="1">
+        <f>0.5*(C26+E26)*(D26-B26)</f>
+        <v>494.86999999999995</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3819</v>
+      </c>
+      <c r="H26" s="1">
+        <f>G26-F26</f>
+        <v>3324.13</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H1048576" s="1"/>
+      <c r="I1048576" s="1"/>
+      <c r="J1048576" s="1"/>
+      <c r="K1048576" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:T15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.08</v>
+      </c>
+      <c r="E3">
+        <f>($T$6*$T$8*$T$8)/(4*PI()*C3*$T$9*($T$8*$T$8-$T$7))*(EXP(-C3/$T$8)-EXP(-C3/SQRT($T$7)))</f>
+        <v>26626537709.542053</v>
+      </c>
+      <c r="F3">
+        <v>3476970.5</v>
+      </c>
+      <c r="G3">
+        <f>F3/(600*0.17*0.024)</f>
+        <v>1420331.0866013069</v>
+      </c>
+      <c r="H3">
+        <f>SQRT(G3)</f>
+        <v>1191.7764415364597</v>
+      </c>
+      <c r="I3">
+        <f>((G3-E3)/H3)^2</f>
+        <v>499106780175347.25</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E13" si="0">($T$6*$T$8*$T$8)/(4*PI()*C4*$T$9*($T$8*$T$8-$T$7))*(EXP(-C4/$T$8)-EXP(-C4/SQRT($T$7)))</f>
+        <v>26037190345.94352</v>
+      </c>
+      <c r="F4">
+        <v>2824068</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G13" si="1">F4/(600*0.17*0.024)</f>
+        <v>1153622.5490196077</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H13" si="2">SQRT(G4)</f>
+        <v>1074.0682236336795</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I13" si="3">((G4-E4)/H4)^2</f>
+        <v>587605719772061.5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>0.12</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>25462986588.098873</v>
+      </c>
+      <c r="F5">
+        <v>2128958</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>869672.38562091487</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>932.56226903135791</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>745475432529198.12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>24903497718.727978</v>
+      </c>
+      <c r="F6">
+        <v>1502338.4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>613700.32679738547</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>783.39027744629652</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>1010515401988185.7</v>
+      </c>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="10">
+        <v>36000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>0.16</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>24358307933.375008</v>
+      </c>
+      <c r="F7">
+        <v>1058639.2</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>432450.65359477117</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>657.60980345093026</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>1371962542083980.2</v>
+      </c>
+      <c r="S7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T7" s="7">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>0.18</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>23827013935.160118</v>
+      </c>
+      <c r="F8">
+        <v>749202</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>306046.56862745091</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>553.21475814321047</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>1854985701536622.2</v>
+      </c>
+      <c r="S8" t="s">
+        <v>40</v>
+      </c>
+      <c r="T8" s="7">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="9" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>23309224542.61937</v>
+      </c>
+      <c r="F9">
+        <v>527716.01500000001</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>215570.26756535945</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>464.29545288033938</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>2520337824920354</v>
+      </c>
+      <c r="S9" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" s="7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.22</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>22804560310.201843</v>
+      </c>
+      <c r="F10">
+        <v>363652.89</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>148551.01715686274</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>385.42316634689041</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>3500758228624595</v>
+      </c>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.24</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>22312653161.0061</v>
+      </c>
+      <c r="F11">
+        <v>256229.14</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>104668.76633986927</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>323.52552656609532</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>4756431528026098</v>
+      </c>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0.26</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>21833146031.353085</v>
+      </c>
+      <c r="F12">
+        <v>179863.58</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>73473.684640522857</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>271.06029705680407</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>6487806615941927</v>
+      </c>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>21365692526.805603</v>
+      </c>
+      <c r="F13">
+        <v>127430.54</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>52054.959150326787</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>228.15555910458721</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>8769396811049795</v>
+      </c>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="H15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="9">
+        <f>SUM(I3:I13)</f>
+        <v>3.2104382586648164E+16</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>